<commit_message>
Uniandes 2023: pulir redacción CV
</commit_message>
<xml_diff>
--- a/Especial_Uniandes_2023/1. CV/data/service_es.xlsx
+++ b/Especial_Uniandes_2023/1. CV/data/service_es.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\Especial_Uniandes_2023\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\Especial_Uniandes_2023\1. CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971F9F2B-EFF5-42E0-8775-D6C14D857D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3944F341-FED7-4073-AABF-5CC27CDBF7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="3030" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -82,12 +82,6 @@
     <t>Desde 2023</t>
   </si>
   <si>
-    <t>Emisión de recomendaciones de las fases 1 y 2</t>
-  </si>
-  <si>
-    <t>Perfil \href{https://rr.peercommunityin.org/public/user_public_page?userId=1996}{Recommender}</t>
-  </si>
-  <si>
     <t>Comité Editorial invitado</t>
   </si>
   <si>
@@ -98,6 +92,12 @@
   </si>
   <si>
     <t>\space</t>
+  </si>
+  <si>
+    <t>Asignación de pares, evaluación de propuestas y emisión de recomendaciones de las fases 1 y 2 de \href{https://www.cos.io/initiatives/registered-reports}{reportes registrados}</t>
+  </si>
+  <si>
+    <t>Perfil como \href{https://rr.peercommunityin.org/public/user_public_page?userId=1996}{recomendador}</t>
   </si>
 </sst>
 </file>
@@ -943,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3AFA9E8-48DD-493D-A757-B362F16614DE}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,12 +988,12 @@
         <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1007,7 +1007,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -1045,13 +1045,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>